<commit_message>
Stand doc list/detail views. Scoped all list views to stand/plot.
</commit_message>
<xml_diff>
--- a/odk_app/config/tables/stand_doc/forms/stand_doc/stand_doc.xlsx
+++ b/odk_app/config/tables/stand_doc/forms/stand_doc/stand_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\dev\classes\capstone\app-designer-2.1.6\app\config\tables\stand_doc\forms\stand_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B78DDE8-31F8-48A5-99DA-C8FFFA69B2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6845A626-7D54-4A8A-A97F-DDEC79A259B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13635" yWindow="-7980" windowWidth="13080" windowHeight="15060" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5730" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>setting_name</t>
   </si>
@@ -80,9 +80,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>SPREADSHEET</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
@@ -126,6 +123,21 @@
   </si>
   <si>
     <t>stand</t>
+  </si>
+  <si>
+    <t>LIST</t>
+  </si>
+  <si>
+    <t>detailViewFileName</t>
+  </si>
+  <si>
+    <t>listViewFileName</t>
+  </si>
+  <si>
+    <t>config/tables/stand_doc/html/stand_doc_detail.html</t>
+  </si>
+  <si>
+    <t>config/tables/stand_doc/html/stand_doc_list.html</t>
   </si>
 </sst>
 </file>
@@ -624,7 +636,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -642,7 +654,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -652,7 +664,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -667,10 +679,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A68881D-8809-487D-A56B-3A7502CC8B35}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -709,7 +721,41 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -760,65 +806,65 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">

</xml_diff>